<commit_message>
GET API Keyword with JSON scema validation
`GET API Keyword with JSON scema validation
</commit_message>
<xml_diff>
--- a/src/main/java/com/cdp/InputFiles/API.xlsx
+++ b/src/main/java/com/cdp/InputFiles/API.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="345" windowWidth="20730" windowHeight="9705" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="345" windowWidth="14790" windowHeight="6720" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
     <sheet name="TestSteps" sheetId="2" r:id="rId2"/>
     <sheet name="CDPLogin" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="API" sheetId="4" r:id="rId4"/>
+    <sheet name="DELETEAPI" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="106">
   <si>
     <t>Proceed_ON_FAIL</t>
   </si>
@@ -38,9 +39,6 @@
   </si>
   <si>
     <t>Target</t>
-  </si>
-  <si>
-    <t>OpenWebApp</t>
   </si>
   <si>
     <t>TS01</t>
@@ -79,9 +77,6 @@
     <t>TS02</t>
   </si>
   <si>
-    <t>Can the user launches the web application?</t>
-  </si>
-  <si>
     <t>TS03</t>
   </si>
   <si>
@@ -311,22 +306,40 @@
     <t>GETAPI</t>
   </si>
   <si>
-    <t>created</t>
-  </si>
-  <si>
-    <t>arg0</t>
-  </si>
-  <si>
-    <t>arg0Type</t>
-  </si>
-  <si>
-    <t>String</t>
-  </si>
-  <si>
-    <t>Mandate</t>
-  </si>
-  <si>
-    <t>Yes</t>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>http://52.221.32.110/dsapi/v1/LayoutsConfigs</t>
+  </si>
+  <si>
+    <t>Content-Type</t>
+  </si>
+  <si>
+    <t>application/json</t>
+  </si>
+  <si>
+    <t>Authorization</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>Validate GET API</t>
+  </si>
+  <si>
+    <t>GetAPIScema</t>
+  </si>
+  <si>
+    <t>DELETEAPI</t>
+  </si>
+  <si>
+    <t>Delete API</t>
+  </si>
+  <si>
+    <t>Validate Delete API</t>
+  </si>
+  <si>
+    <t>http://52.221.32.110/dsapi/v1/LayoutsConfigs/59ca2542dd14286f3bb89eb9</t>
   </si>
 </sst>
 </file>
@@ -494,7 +507,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -511,6 +524,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -874,10 +888,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -889,30 +903,44 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -927,7 +955,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -944,22 +972,22 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>1</v>
@@ -968,88 +996,88 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1">
       <c r="A2" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>95</v>
-      </c>
       <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="F2" s="5" t="s">
+        <v>101</v>
+      </c>
       <c r="G2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="7" t="s">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>19</v>
+        <v>104</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>42</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>38</v>
+      <c r="H3" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -1057,249 +1085,249 @@
         <v>2</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="11"/>
@@ -1307,55 +1335,55 @@
         <v>2</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1">
       <c r="A17" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>42</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9" t="s">
         <v>2</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1369,7 +1397,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1385,110 +1415,110 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" s="12" t="s">
+      <c r="F1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1498,37 +1528,133 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
         <v>97</v>
       </c>
-      <c r="B1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" t="s">
-        <v>99</v>
+        <v>70</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Driver Script & Configs updated to store Centralized HTML Reports
</commit_message>
<xml_diff>
--- a/src/main/java/com/cdp/InputFiles/API.xlsx
+++ b/src/main/java/com/cdp/InputFiles/API.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="345" windowWidth="14790" windowHeight="6720" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="345" windowWidth="14790" windowHeight="6720"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
     <sheet name="TestSteps" sheetId="2" r:id="rId2"/>
     <sheet name="GET" sheetId="4" r:id="rId3"/>
-    <sheet name="DELETEAPI" sheetId="5" r:id="rId4"/>
-    <sheet name="POST" sheetId="6" r:id="rId5"/>
+    <sheet name="POST" sheetId="6" r:id="rId4"/>
+    <sheet name="DELETEAPI" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="59">
   <si>
     <t>Proceed_ON_FAIL</t>
   </si>
@@ -45,10 +45,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>YES</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>TCID</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -80,100 +76,10 @@
     <t>TS04</t>
   </si>
   <si>
-    <t>Click</t>
-  </si>
-  <si>
-    <t>resetApp</t>
-  </si>
-  <si>
-    <t>TS07</t>
-  </si>
-  <si>
-    <t>verifyText</t>
-  </si>
-  <si>
-    <t>TS08</t>
-  </si>
-  <si>
-    <t>TS09</t>
-  </si>
-  <si>
-    <t>TS10</t>
-  </si>
-  <si>
-    <t>TS11</t>
-  </si>
-  <si>
-    <t>TS12</t>
-  </si>
-  <si>
-    <t>TS13</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Reset web application</t>
-  </si>
-  <si>
-    <t>CDPLogin</t>
-  </si>
-  <si>
-    <t>CDP_URL</t>
-  </si>
-  <si>
     <t>YES</t>
-  </si>
-  <si>
-    <t>validate CDP welcome message text</t>
-  </si>
-  <si>
-    <t>WelcomeMessage</t>
-  </si>
-  <si>
-    <t>Forgot your password?</t>
-  </si>
-  <si>
-    <t>validate Forgot password link text</t>
-  </si>
-  <si>
-    <t>ForgotPasswordLink</t>
-  </si>
-  <si>
-    <t>NewCustomerRegistrationLink</t>
-  </si>
-  <si>
-    <t>validate New Customer Registration Link text</t>
-  </si>
-  <si>
-    <t>New Customer Registration</t>
-  </si>
-  <si>
-    <t>Sign In</t>
-  </si>
-  <si>
-    <t>validate Sign In button text</t>
-  </si>
-  <si>
-    <t>SignInButton</t>
-  </si>
-  <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>Input user name in User Name Field</t>
-  </si>
-  <si>
-    <t>Input password in password field</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Click on Sign In button</t>
   </si>
   <si>
     <t>DSID</t>
@@ -192,42 +98,6 @@
     <t>DS01</t>
   </si>
   <si>
-    <t>col$Password</t>
-  </si>
-  <si>
-    <t>col$UserName</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>WELCOME TO POLAND</t>
-  </si>
-  <si>
-    <t>verifySignIn</t>
-  </si>
-  <si>
-    <t>verifyErrorMsg</t>
-  </si>
-  <si>
-    <t>validate verify sign in functionality</t>
-  </si>
-  <si>
-    <t>validate error message</t>
-  </si>
-  <si>
-    <t>col$Expectedmsg</t>
-  </si>
-  <si>
-    <t>TS14</t>
-  </si>
-  <si>
-    <t>TS15</t>
-  </si>
-  <si>
-    <t>LoginAlerMessage</t>
-  </si>
-  <si>
     <t>GET API</t>
   </si>
   <si>
@@ -249,9 +119,6 @@
     <t>DELETEAPI</t>
   </si>
   <si>
-    <t>Delete API</t>
-  </si>
-  <si>
     <t>Validate Delete API</t>
   </si>
   <si>
@@ -331,12 +198,6 @@
   </si>
   <si>
     <t>/cdp/v1/policy</t>
-  </si>
-  <si>
-    <t>{"Query":{"Find":{"TriggerActionTemplate":{"sid":{"ne":""}}}}}</t>
-  </si>
-  <si>
-    <t>Events</t>
   </si>
 </sst>
 </file>
@@ -426,7 +287,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -504,6 +365,17 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -525,13 +397,13 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -895,10 +767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -910,86 +782,44 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1001,62 +831,62 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A1" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -1064,21 +894,21 @@
         <v>2</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -1086,21 +916,21 @@
         <v>2</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>101</v>
+        <v>32</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>78</v>
+        <v>31</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -1108,21 +938,21 @@
         <v>2</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>81</v>
+        <v>37</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1130,289 +960,29 @@
         <v>2</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A6" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="3"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="H6" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A17" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1427,7 +997,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1442,128 +1012,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="8" t="s">
+      <c r="A1" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>54</v>
+      <c r="B1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>92</v>
+        <v>42</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>93</v>
+        <v>43</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>94</v>
+        <v>44</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>95</v>
+        <v>45</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>96</v>
+        <v>46</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>93</v>
+        <v>47</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1581,6 +1151,80 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="http://52.221.32.110/dsapi/v1/LayoutsConfigs"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1598,37 +1242,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>54</v>
+      <c r="A1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>77</v>
+        <v>24</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1637,99 +1281,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="C3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://52.221.32.110/dsapi/v1/LayoutsConfigs"/>
-    <hyperlink ref="B3" r:id="rId2" display="http://52.221.32.110/dsapi/v1/LayoutsConfigs"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>